<commit_message>
Updated one to 10^12
</commit_message>
<xml_diff>
--- a/Missing Curvatures.xlsx
+++ b/Missing Curvatures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAMES\Documents\Math\Programs\Apollonian\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ADCAD2-5941-44D0-B0C6-996FE17D45A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC805A9-22ED-4E32-9AB4-0CCDFA3E9AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="0" windowWidth="22944" windowHeight="12240" tabRatio="775" activeTab="1" xr2:uid="{8C34F5AD-CAF7-48CF-A3DC-CD7011562DF6}"/>
+    <workbookView xWindow="96" yWindow="0" windowWidth="22944" windowHeight="12240" tabRatio="775" activeTab="8" xr2:uid="{8C34F5AD-CAF7-48CF-A3DC-CD7011562DF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="12" r:id="rId1"/>
@@ -23460,9 +23460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE4644-CCC9-4D36-83D5-F9AE01BDCF6A}">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="M20" sqref="A18:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36494,9 +36494,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9951D164-36E6-42AB-B42D-6BFF47135181}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37049,8 +37049,8 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="1">
-        <f>3*10^11</f>
-        <v>300000000000</v>
+        <f>10^12</f>
+        <v>1000000000000</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>428</v>
@@ -37132,7 +37132,7 @@
       </c>
       <c r="K21" s="3">
         <f>B19/J21</f>
-        <v>11.11809678426884</v>
+        <v>37.060322614229463</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">

</xml_diff>